<commit_message>
Added molex B8 connector to library and parts naming sheet
</commit_message>
<xml_diff>
--- a/PartsNaming.xlsx
+++ b/PartsNaming.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winnie\Documents\GitHub\KiCAD_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9CE82B-EFF8-4C04-9979-ED9A0D400C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C69F24-6F88-43CA-818B-D83BBF063D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F328AE42-CB93-44D6-A110-F6DC4C089AB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{F328AE42-CB93-44D6-A110-F6DC4C089AB6}"/>
   </bookViews>
   <sheets>
     <sheet name="JST" sheetId="3" r:id="rId1"/>
-    <sheet name="Molex" sheetId="2" r:id="rId2"/>
-    <sheet name="Resistors" sheetId="5" r:id="rId3"/>
-    <sheet name="JST Data" sheetId="4" r:id="rId4"/>
-    <sheet name="Molex Data" sheetId="1" r:id="rId5"/>
+    <sheet name="LCSC Wishlist" sheetId="6" r:id="rId2"/>
+    <sheet name="Molex Board-Board" sheetId="9" r:id="rId3"/>
+    <sheet name="Molex Wire-Wire" sheetId="2" r:id="rId4"/>
+    <sheet name="Resistors" sheetId="5" r:id="rId5"/>
+    <sheet name="JST Data" sheetId="4" r:id="rId6"/>
+    <sheet name="Molex Data" sheetId="1" r:id="rId7"/>
+    <sheet name="Mezzamine Data" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>Family Name</t>
   </si>
@@ -157,9 +160,6 @@
     <t>JST-SM</t>
   </si>
   <si>
-    <t>X2011</t>
-  </si>
-  <si>
     <t>X2521</t>
   </si>
   <si>
@@ -227,6 +227,51 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Customer Ref.</t>
+  </si>
+  <si>
+    <t>C151885</t>
+  </si>
+  <si>
+    <t>X2000</t>
+  </si>
+  <si>
+    <t>X9396</t>
+  </si>
+  <si>
+    <t>JST-VH</t>
+  </si>
+  <si>
+    <t>Molex B8</t>
+  </si>
+  <si>
+    <t>Plug</t>
+  </si>
+  <si>
+    <t>Socket</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Molex Mezzamine Connectors</t>
+  </si>
+  <si>
+    <t>Total Pins</t>
+  </si>
+  <si>
+    <t>YXT-BB10-</t>
   </si>
 </sst>
 </file>
@@ -610,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF63EB9-3D30-493D-AAF7-7A6EBB36005F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="156" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,15 +694,15 @@
       </c>
       <c r="E3" t="str">
         <f xml:space="preserve"> "Pins/Row" &amp;IF($B$7="T", " (N/A)","")</f>
-        <v>Pins/Row (N/A)</v>
+        <v>Pins/Row</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -677,11 +722,11 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>VLOOKUP(A4, 'JST Data'!A2:B13, 2,FALSE)</f>
-        <v>X2521</v>
+        <v>X2000</v>
       </c>
       <c r="B7" t="str">
         <f>IF('Molex Data'!E2 = JST!B4, 'Molex Data'!D2,IF('Molex Data'!E3 = JST!B4, 'Molex Data'!D3,IF('Molex Data'!E4 = JST!B4, 'Molex Data'!D4)))</f>
-        <v>T</v>
+        <v>H</v>
       </c>
       <c r="C7" t="str">
         <f>IF(B7="W",IF(C4='JST Data'!G2,'JST Data'!H2,IF(C4='JST Data'!G3,'JST Data'!H3,)),"")</f>
@@ -693,7 +738,7 @@
       </c>
       <c r="E7" s="2" t="str">
         <f>IF(B7="T", "", "-"&amp;E4)</f>
-        <v/>
+        <v>-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -704,7 +749,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>A7&amp;B7&amp;C7&amp;D7&amp;TEXT(E7, "00")</f>
-        <v>X2521T</v>
+        <v>X2000H-04</v>
       </c>
     </row>
   </sheetData>
@@ -744,11 +789,147 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF7CC0A-5E12-42DE-AABD-7DF8AD1C753F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAB9FF5-FE60-4BEA-B505-8C98225AD970}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="156" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>VLOOKUP(A4,'Mezzamine Data'!A2:B23, 2, FALSE)</f>
+        <v>YXT-BB10-</v>
+      </c>
+      <c r="B7" s="2">
+        <f>B4</f>
+        <v>10</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(C4,'Mezzamine Data'!D1:E2, 2, FALSE)</f>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>A7&amp;TEXT(B7, "00") &amp;C7</f>
+        <v>YXT-BB10-10S</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Total pins must be even" prompt="Total pins must be even_x000a_" sqref="B4" xr:uid="{89F1B984-8228-429B-ADED-D42D92AF98BA}">
+      <formula1>NOT(MOD(B4,2))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4AD5CBA5-B9C9-4244-B01B-A3C714BB5D16}">
+          <x14:formula1>
+            <xm:f>'Mezzamine Data'!$D$1:$D$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{659D8278-14D4-44C6-973B-43FB2FC62B54}">
+          <x14:formula1>
+            <xm:f>'Mezzamine Data'!$A$2:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36119DCB-3468-4F81-AF1F-52F6E3A3DE06}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,7 +968,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -810,10 +991,10 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>VLOOKUP(A4, 'Molex Data'!A2:B12, 2, FALSE)</f>
-        <v>X3025</v>
+        <v>X9357</v>
       </c>
       <c r="B7" t="str">
-        <f>IF('Molex Data'!E2 = Molex!B4, 'Molex Data'!D2,IF('Molex Data'!E3 = Molex!B4, 'Molex Data'!D3,IF('Molex Data'!E4 = Molex!B4, 'Molex Data'!D4)))</f>
+        <f>IF('Molex Data'!E2 = 'Molex Wire-Wire'!B4, 'Molex Data'!D2,IF('Molex Data'!E3 = 'Molex Wire-Wire'!B4, 'Molex Data'!D3,IF('Molex Data'!E4 = 'Molex Wire-Wire'!B4, 'Molex Data'!D4)))</f>
         <v>H</v>
       </c>
       <c r="C7" t="str">
@@ -837,7 +1018,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>A7&amp;B7&amp;C7&amp;D7&amp;TEXT(E7, "00")</f>
-        <v>X3025HM-2x05</v>
+        <v>X9357HM-2x05</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +1033,7 @@
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C6F6BB79-DB0B-49C4-AE9B-8303480F378A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{107DB8B2-FF8A-426F-B24B-1F1463B3D7F3}">
           <x14:formula1>
             <xm:f>'Molex Data'!$A$2:$A$10</xm:f>
           </x14:formula1>
@@ -870,7 +1051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FA13AB-9CFB-42B8-9BA0-228E33BAB919}">
   <dimension ref="A1:V10"/>
   <sheetViews>
@@ -888,34 +1069,34 @@
   <sheetData>
     <row r="1" spans="1:22" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
         <v>6</v>
       </c>
       <c r="O1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T1" s="4">
         <v>1005</v>
       </c>
       <c r="U1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="23.4" x14ac:dyDescent="0.45">
@@ -933,13 +1114,13 @@
         <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O2">
         <v>-1</v>
       </c>
       <c r="Q2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R2" s="5">
         <v>5.0000000000000001E-3</v>
@@ -948,15 +1129,15 @@
         <v>201</v>
       </c>
       <c r="U2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O3">
         <v>-2</v>
@@ -971,10 +1152,10 @@
         <v>402</v>
       </c>
       <c r="U3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
@@ -999,13 +1180,13 @@
         <v>J</v>
       </c>
       <c r="N4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O4">
         <v>-3</v>
       </c>
       <c r="Q4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R4" s="6">
         <v>0.02</v>
@@ -1014,15 +1195,15 @@
         <v>603</v>
       </c>
       <c r="U4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="Q5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R5" s="6">
         <v>0.05</v>
@@ -1031,10 +1212,10 @@
         <v>805</v>
       </c>
       <c r="U5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="25.8" x14ac:dyDescent="0.5">
@@ -1046,10 +1227,10 @@
         <v>1206</v>
       </c>
       <c r="U6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -1078,12 +1259,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7E1101-C29D-4CE6-8BA4-B780D5856F91}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,7 +1295,7 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1164,11 +1345,11 @@
       </c>
       <c r="D4" t="str">
         <f>IF(JST!$A$4="JST-SM", "", "W")</f>
-        <v/>
+        <v>W</v>
       </c>
       <c r="E4" t="str">
         <f>IF(JST!$A$4="JST-SM", "", "Board Mounted Connector")</f>
-        <v/>
+        <v>Board Mounted Connector</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
@@ -1187,7 +1368,15 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAD1FF-20A4-4F87-9F74-5BE9A600175B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1277,4 +1466,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2142F3-EE28-474E-8328-93E41BE8217A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="70.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>